<commit_message>
2d vs 1d arrays with 2015 vs 2017 matlab versions
</commit_message>
<xml_diff>
--- a/matlabOverhangFinder/Accompanying Excel Workbook_BACKUP.xlsx
+++ b/matlabOverhangFinder/Accompanying Excel Workbook_BACKUP.xlsx
@@ -2360,20 +2360,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="72" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="74" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2384,34 +2376,43 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="72" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="74" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="79" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="80" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2432,23 +2433,22 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="74" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2473,7 +2473,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="72" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="74" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="79" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="81" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="80" xfId="2" applyBorder="1" applyAlignment="1">
@@ -2485,37 +2494,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="72" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="73" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="74" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2543,7 +2527,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="81" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="73" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3284,7 +3284,7 @@
   <dimension ref="A1:AW74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="H12" sqref="H12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,14 +3314,14 @@
       <c r="A2" s="107"/>
       <c r="B2" s="113"/>
       <c r="C2" s="114"/>
-      <c r="D2" s="174" t="s">
+      <c r="D2" s="173" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
-      <c r="I2" s="174"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
+      <c r="H2" s="173"/>
+      <c r="I2" s="173"/>
       <c r="J2" s="115"/>
       <c r="K2" s="116"/>
     </row>
@@ -3329,12 +3329,12 @@
       <c r="A3" s="107"/>
       <c r="B3" s="117"/>
       <c r="C3" s="118"/>
-      <c r="D3" s="175"/>
-      <c r="E3" s="175"/>
-      <c r="F3" s="175"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="175"/>
-      <c r="I3" s="175"/>
+      <c r="D3" s="174"/>
+      <c r="E3" s="174"/>
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="174"/>
       <c r="J3" s="119"/>
       <c r="K3" s="116"/>
     </row>
@@ -3342,14 +3342,14 @@
       <c r="A4" s="107"/>
       <c r="B4" s="120"/>
       <c r="C4" s="121"/>
-      <c r="D4" s="176" t="s">
+      <c r="D4" s="177" t="s">
         <v>177</v>
       </c>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="178"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="179"/>
       <c r="J4" s="122"/>
       <c r="K4" s="116"/>
     </row>
@@ -3357,25 +3357,25 @@
       <c r="A5" s="107"/>
       <c r="B5" s="120"/>
       <c r="C5" s="116"/>
-      <c r="D5" s="179" t="s">
+      <c r="D5" s="180" t="s">
         <v>241</v>
       </c>
-      <c r="E5" s="180"/>
-      <c r="F5" s="180"/>
-      <c r="G5" s="180"/>
-      <c r="H5" s="180"/>
-      <c r="I5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="182"/>
       <c r="J5" s="122"/>
       <c r="K5" s="116"/>
       <c r="L5" s="108" t="s">
         <v>247</v>
       </c>
-      <c r="M5" s="182"/>
-      <c r="N5" s="182"/>
-      <c r="O5" s="182"/>
-      <c r="P5" s="182"/>
-      <c r="Q5" s="182"/>
-      <c r="R5" s="182"/>
+      <c r="M5" s="158"/>
+      <c r="N5" s="158"/>
+      <c r="O5" s="158"/>
+      <c r="P5" s="158"/>
+      <c r="Q5" s="158"/>
+      <c r="R5" s="158"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="107"/>
@@ -3393,16 +3393,16 @@
       <c r="C7" s="123" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="163" t="s">
+      <c r="D7" s="161" t="s">
         <v>246</v>
       </c>
-      <c r="E7" s="164"/>
-      <c r="F7" s="164"/>
-      <c r="G7" s="166"/>
-      <c r="H7" s="170" t="s">
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="183"/>
+      <c r="H7" s="175" t="s">
         <v>240</v>
       </c>
-      <c r="I7" s="171"/>
+      <c r="I7" s="176"/>
       <c r="J7" s="122"/>
       <c r="K7" s="116"/>
       <c r="N7" s="124"/>
@@ -3426,16 +3426,16 @@
       <c r="C9" s="123" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="163" t="s">
+      <c r="D9" s="161" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="173"/>
-      <c r="H9" s="161">
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="164">
         <v>3</v>
       </c>
-      <c r="I9" s="162"/>
+      <c r="I9" s="165"/>
       <c r="J9" s="122"/>
       <c r="K9" s="116"/>
     </row>
@@ -3458,16 +3458,16 @@
       <c r="C11" s="123" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="163" t="s">
+      <c r="D11" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="164"/>
-      <c r="F11" s="164"/>
-      <c r="G11" s="165"/>
-      <c r="H11" s="170">
+      <c r="E11" s="162"/>
+      <c r="F11" s="162"/>
+      <c r="G11" s="163"/>
+      <c r="H11" s="175">
         <v>23</v>
       </c>
-      <c r="I11" s="171"/>
+      <c r="I11" s="176"/>
       <c r="J11" s="122"/>
       <c r="K11" s="116"/>
     </row>
@@ -3475,16 +3475,16 @@
       <c r="A12" s="107"/>
       <c r="B12" s="120"/>
       <c r="C12" s="123"/>
-      <c r="D12" s="163" t="s">
+      <c r="D12" s="161" t="s">
         <v>178</v>
       </c>
-      <c r="E12" s="164"/>
-      <c r="F12" s="164"/>
-      <c r="G12" s="165"/>
-      <c r="H12" s="170">
-        <v>22</v>
-      </c>
-      <c r="I12" s="171"/>
+      <c r="E12" s="162"/>
+      <c r="F12" s="162"/>
+      <c r="G12" s="163"/>
+      <c r="H12" s="175">
+        <v>1</v>
+      </c>
+      <c r="I12" s="176"/>
       <c r="J12" s="122"/>
       <c r="K12" s="116"/>
     </row>
@@ -3501,16 +3501,16 @@
       <c r="C14" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="163" t="s">
+      <c r="D14" s="161" t="s">
         <v>242</v>
       </c>
-      <c r="E14" s="164"/>
-      <c r="F14" s="164"/>
-      <c r="G14" s="164"/>
-      <c r="H14" s="161" t="s">
+      <c r="E14" s="162"/>
+      <c r="F14" s="162"/>
+      <c r="G14" s="162"/>
+      <c r="H14" s="164" t="s">
         <v>245</v>
       </c>
-      <c r="I14" s="162"/>
+      <c r="I14" s="165"/>
       <c r="J14" s="122"/>
       <c r="K14" s="116"/>
     </row>
@@ -3526,16 +3526,16 @@
       <c r="C16" s="123" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="163" t="s">
+      <c r="D16" s="161" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="164"/>
-      <c r="F16" s="164"/>
-      <c r="G16" s="166"/>
-      <c r="H16" s="161">
+      <c r="E16" s="162"/>
+      <c r="F16" s="162"/>
+      <c r="G16" s="183"/>
+      <c r="H16" s="164">
         <v>2</v>
       </c>
-      <c r="I16" s="162"/>
+      <c r="I16" s="165"/>
       <c r="J16" s="122"/>
       <c r="K16" s="116"/>
     </row>
@@ -3543,12 +3543,12 @@
       <c r="A17" s="107"/>
       <c r="B17" s="120"/>
       <c r="C17" s="123"/>
-      <c r="D17" s="163" t="s">
+      <c r="D17" s="161" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="164"/>
-      <c r="F17" s="164"/>
-      <c r="G17" s="165"/>
+      <c r="E17" s="162"/>
+      <c r="F17" s="162"/>
+      <c r="G17" s="163"/>
       <c r="J17" s="130"/>
       <c r="K17" s="116"/>
     </row>
@@ -3571,16 +3571,16 @@
       <c r="C19" s="128" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="158" t="s">
+      <c r="D19" s="171" t="s">
         <v>175</v>
       </c>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="161">
+      <c r="E19" s="172"/>
+      <c r="F19" s="172"/>
+      <c r="G19" s="172"/>
+      <c r="H19" s="164">
         <v>1</v>
       </c>
-      <c r="I19" s="162"/>
+      <c r="I19" s="165"/>
       <c r="J19" s="122"/>
       <c r="K19" s="116"/>
     </row>
@@ -3588,12 +3588,12 @@
       <c r="A20" s="107"/>
       <c r="B20" s="120"/>
       <c r="C20" s="128"/>
-      <c r="D20" s="163" t="s">
+      <c r="D20" s="161" t="s">
         <v>176</v>
       </c>
-      <c r="E20" s="164"/>
-      <c r="F20" s="164"/>
-      <c r="G20" s="165"/>
+      <c r="E20" s="162"/>
+      <c r="F20" s="162"/>
+      <c r="G20" s="163"/>
       <c r="H20" s="112"/>
       <c r="I20" s="112"/>
       <c r="J20" s="122"/>
@@ -3606,12 +3606,12 @@
       <c r="A21" s="107"/>
       <c r="B21" s="120"/>
       <c r="C21" s="128"/>
-      <c r="D21" s="163" t="s">
+      <c r="D21" s="161" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="164"/>
-      <c r="F21" s="164"/>
-      <c r="G21" s="165"/>
+      <c r="E21" s="162"/>
+      <c r="F21" s="162"/>
+      <c r="G21" s="163"/>
       <c r="H21" s="112"/>
       <c r="I21" s="112"/>
       <c r="J21" s="130"/>
@@ -3621,10 +3621,10 @@
       <c r="A22" s="107"/>
       <c r="B22" s="120"/>
       <c r="C22" s="123"/>
-      <c r="D22" s="163"/>
-      <c r="E22" s="164"/>
-      <c r="F22" s="164"/>
-      <c r="G22" s="164"/>
+      <c r="D22" s="161"/>
+      <c r="E22" s="162"/>
+      <c r="F22" s="162"/>
+      <c r="G22" s="162"/>
       <c r="H22" s="112"/>
       <c r="I22" s="112"/>
       <c r="J22" s="122"/>
@@ -3639,16 +3639,16 @@
       <c r="C23" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="163" t="s">
+      <c r="D23" s="161" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="164"/>
-      <c r="F23" s="164"/>
-      <c r="G23" s="173"/>
-      <c r="H23" s="161">
+      <c r="E23" s="162"/>
+      <c r="F23" s="162"/>
+      <c r="G23" s="170"/>
+      <c r="H23" s="164">
         <v>2</v>
       </c>
-      <c r="I23" s="162"/>
+      <c r="I23" s="165"/>
       <c r="J23" s="130"/>
       <c r="K23" s="116"/>
     </row>
@@ -3656,12 +3656,12 @@
       <c r="A24" s="107"/>
       <c r="B24" s="120"/>
       <c r="C24" s="132"/>
-      <c r="D24" s="163" t="s">
+      <c r="D24" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="164"/>
-      <c r="F24" s="164"/>
-      <c r="G24" s="165"/>
+      <c r="E24" s="162"/>
+      <c r="F24" s="162"/>
+      <c r="G24" s="163"/>
       <c r="H24" s="112"/>
       <c r="I24" s="112"/>
       <c r="J24" s="122"/>
@@ -3679,16 +3679,16 @@
       <c r="C26" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="158" t="s">
+      <c r="D26" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="159"/>
-      <c r="F26" s="159"/>
-      <c r="G26" s="172"/>
-      <c r="H26" s="161">
+      <c r="E26" s="172"/>
+      <c r="F26" s="172"/>
+      <c r="G26" s="184"/>
+      <c r="H26" s="164">
         <v>1</v>
       </c>
-      <c r="I26" s="162"/>
+      <c r="I26" s="165"/>
       <c r="J26" s="134"/>
       <c r="K26" s="116"/>
     </row>
@@ -3696,12 +3696,12 @@
       <c r="A27" s="107"/>
       <c r="B27" s="133"/>
       <c r="C27" s="136"/>
-      <c r="D27" s="163" t="s">
+      <c r="D27" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="164"/>
-      <c r="F27" s="164"/>
-      <c r="G27" s="164"/>
+      <c r="E27" s="162"/>
+      <c r="F27" s="162"/>
+      <c r="G27" s="162"/>
       <c r="J27" s="134"/>
       <c r="K27" s="116"/>
     </row>
@@ -3722,14 +3722,14 @@
       <c r="A29" s="107"/>
       <c r="B29" s="113"/>
       <c r="C29" s="114"/>
-      <c r="D29" s="174" t="s">
+      <c r="D29" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="174"/>
-      <c r="F29" s="174"/>
-      <c r="G29" s="174"/>
-      <c r="H29" s="174"/>
-      <c r="I29" s="174"/>
+      <c r="E29" s="173"/>
+      <c r="F29" s="173"/>
+      <c r="G29" s="173"/>
+      <c r="H29" s="173"/>
+      <c r="I29" s="173"/>
       <c r="J29" s="115"/>
       <c r="K29" s="116"/>
     </row>
@@ -3737,12 +3737,12 @@
       <c r="A30" s="107"/>
       <c r="B30" s="117"/>
       <c r="C30" s="118"/>
-      <c r="D30" s="175"/>
-      <c r="E30" s="175"/>
-      <c r="F30" s="175"/>
-      <c r="G30" s="175"/>
-      <c r="H30" s="175"/>
-      <c r="I30" s="175"/>
+      <c r="D30" s="174"/>
+      <c r="E30" s="174"/>
+      <c r="F30" s="174"/>
+      <c r="G30" s="174"/>
+      <c r="H30" s="174"/>
+      <c r="I30" s="174"/>
       <c r="J30" s="119"/>
       <c r="K30" s="116"/>
     </row>
@@ -3752,13 +3752,13 @@
       <c r="D31" s="135" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="167" t="s">
+      <c r="E31" s="186" t="s">
         <v>243</v>
       </c>
-      <c r="F31" s="168"/>
-      <c r="G31" s="168"/>
-      <c r="H31" s="168"/>
-      <c r="I31" s="169"/>
+      <c r="F31" s="187"/>
+      <c r="G31" s="187"/>
+      <c r="H31" s="187"/>
+      <c r="I31" s="188"/>
       <c r="J31" s="122"/>
       <c r="K31" s="116"/>
       <c r="L31" s="112"/>
@@ -4029,13 +4029,13 @@
       <c r="D49" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="185" t="s">
+      <c r="E49" s="166" t="s">
         <v>91</v>
       </c>
-      <c r="F49" s="185"/>
-      <c r="G49" s="185"/>
-      <c r="H49" s="185"/>
-      <c r="I49" s="185"/>
+      <c r="F49" s="166"/>
+      <c r="G49" s="166"/>
+      <c r="H49" s="166"/>
+      <c r="I49" s="166"/>
       <c r="K49" s="114"/>
       <c r="L49" s="150"/>
       <c r="M49" s="150"/>
@@ -4054,13 +4054,13 @@
       <c r="B50" s="152"/>
       <c r="C50" s="153"/>
       <c r="D50" s="153"/>
-      <c r="E50" s="186" t="s">
+      <c r="E50" s="167" t="s">
         <v>244</v>
       </c>
-      <c r="F50" s="187"/>
-      <c r="G50" s="187"/>
-      <c r="H50" s="187"/>
-      <c r="I50" s="188"/>
+      <c r="F50" s="168"/>
+      <c r="G50" s="168"/>
+      <c r="H50" s="168"/>
+      <c r="I50" s="169"/>
       <c r="J50" s="153"/>
       <c r="K50" s="116"/>
       <c r="U50" s="122"/>
@@ -4126,7 +4126,7 @@
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="107"/>
       <c r="B52" s="120"/>
-      <c r="C52" s="183" t="s">
+      <c r="C52" s="159" t="s">
         <v>50</v>
       </c>
       <c r="D52" s="141">
@@ -4160,7 +4160,7 @@
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="107"/>
       <c r="B53" s="120"/>
-      <c r="C53" s="184"/>
+      <c r="C53" s="160"/>
       <c r="D53" s="141">
         <v>2</v>
       </c>
@@ -4579,27 +4579,27 @@
       <c r="D69" s="135" t="s">
         <v>179</v>
       </c>
-      <c r="E69" s="163" t="s">
+      <c r="E69" s="161" t="s">
         <v>49</v>
       </c>
-      <c r="F69" s="164"/>
-      <c r="G69" s="164"/>
-      <c r="H69" s="164"/>
-      <c r="I69" s="173"/>
-      <c r="J69" s="161">
+      <c r="F69" s="162"/>
+      <c r="G69" s="162"/>
+      <c r="H69" s="162"/>
+      <c r="I69" s="170"/>
+      <c r="J69" s="164">
         <v>8</v>
       </c>
-      <c r="K69" s="162"/>
+      <c r="K69" s="165"/>
       <c r="U69" s="122"/>
       <c r="V69" s="116"/>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="107"/>
       <c r="B70" s="120"/>
-      <c r="E70" s="163"/>
-      <c r="F70" s="164"/>
-      <c r="G70" s="164"/>
-      <c r="H70" s="165"/>
+      <c r="E70" s="161"/>
+      <c r="F70" s="162"/>
+      <c r="G70" s="162"/>
+      <c r="H70" s="163"/>
       <c r="U70" s="122"/>
       <c r="V70" s="116"/>
     </row>
@@ -4609,30 +4609,30 @@
       <c r="D71" s="135" t="s">
         <v>180</v>
       </c>
-      <c r="E71" s="158" t="s">
+      <c r="E71" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="F71" s="159"/>
-      <c r="G71" s="159"/>
-      <c r="H71" s="159"/>
-      <c r="I71" s="172"/>
-      <c r="J71" s="161" t="s">
+      <c r="F71" s="172"/>
+      <c r="G71" s="172"/>
+      <c r="H71" s="172"/>
+      <c r="I71" s="184"/>
+      <c r="J71" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="K71" s="162"/>
+      <c r="K71" s="165"/>
       <c r="U71" s="122"/>
       <c r="V71" s="116"/>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="107"/>
       <c r="B72" s="120"/>
-      <c r="E72" s="158" t="s">
+      <c r="E72" s="171" t="s">
         <v>101</v>
       </c>
-      <c r="F72" s="159"/>
-      <c r="G72" s="159"/>
-      <c r="H72" s="159"/>
-      <c r="I72" s="160"/>
+      <c r="F72" s="172"/>
+      <c r="G72" s="172"/>
+      <c r="H72" s="172"/>
+      <c r="I72" s="185"/>
       <c r="U72" s="122"/>
       <c r="V72" s="116"/>
     </row>
@@ -4684,6 +4684,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="E72:I72"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="E71:I71"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D2:I3"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="D7:G7"/>
     <mergeCell ref="M5:R5"/>
     <mergeCell ref="C52:C53"/>
     <mergeCell ref="E70:H70"/>
@@ -4700,29 +4723,6 @@
     <mergeCell ref="D29:I30"/>
     <mergeCell ref="D11:G11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D2:I3"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="E71:I71"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="E72:I72"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="D27:G27"/>
   </mergeCells>
   <conditionalFormatting sqref="E52:G52 E60:T67 E53:E55 G55:J55 F54:F55 G53:G54 I54:J54 J53 E56:K59 M52:T59">
     <cfRule type="notContainsBlanks" dxfId="17" priority="15">
@@ -16246,14 +16246,14 @@
       <c r="A2" s="2"/>
       <c r="B2" s="5"/>
       <c r="C2" s="37"/>
-      <c r="D2" s="202" t="s">
+      <c r="D2" s="204" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="202"/>
-      <c r="F2" s="202"/>
-      <c r="G2" s="202"/>
-      <c r="H2" s="202"/>
-      <c r="I2" s="202"/>
+      <c r="E2" s="204"/>
+      <c r="F2" s="204"/>
+      <c r="G2" s="204"/>
+      <c r="H2" s="204"/>
+      <c r="I2" s="204"/>
       <c r="J2" s="29"/>
       <c r="K2" s="3"/>
     </row>
@@ -16261,12 +16261,12 @@
       <c r="A3" s="2"/>
       <c r="B3" s="30"/>
       <c r="C3" s="38"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="203"/>
-      <c r="F3" s="203"/>
-      <c r="G3" s="203"/>
-      <c r="H3" s="203"/>
-      <c r="I3" s="203"/>
+      <c r="D3" s="205"/>
+      <c r="E3" s="205"/>
+      <c r="F3" s="205"/>
+      <c r="G3" s="205"/>
+      <c r="H3" s="205"/>
+      <c r="I3" s="205"/>
       <c r="J3" s="31"/>
       <c r="K3" s="3"/>
     </row>
@@ -16274,14 +16274,14 @@
       <c r="A4" s="2"/>
       <c r="B4" s="6"/>
       <c r="C4" s="36"/>
-      <c r="D4" s="204" t="s">
+      <c r="D4" s="219" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="205"/>
-      <c r="F4" s="205"/>
-      <c r="G4" s="205"/>
-      <c r="H4" s="205"/>
-      <c r="I4" s="206"/>
+      <c r="E4" s="220"/>
+      <c r="F4" s="220"/>
+      <c r="G4" s="220"/>
+      <c r="H4" s="220"/>
+      <c r="I4" s="221"/>
       <c r="J4" s="7"/>
       <c r="K4" s="3"/>
     </row>
@@ -16289,22 +16289,22 @@
       <c r="A5" s="2"/>
       <c r="B5" s="6"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="207" t="s">
+      <c r="D5" s="197" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="208"/>
-      <c r="F5" s="208"/>
-      <c r="G5" s="208"/>
-      <c r="H5" s="208"/>
-      <c r="I5" s="209"/>
+      <c r="E5" s="215"/>
+      <c r="F5" s="215"/>
+      <c r="G5" s="215"/>
+      <c r="H5" s="215"/>
+      <c r="I5" s="198"/>
       <c r="J5" s="7"/>
       <c r="K5" s="3"/>
-      <c r="M5" s="211"/>
-      <c r="N5" s="211"/>
-      <c r="O5" s="211"/>
-      <c r="P5" s="211"/>
-      <c r="Q5" s="211"/>
-      <c r="R5" s="211"/>
+      <c r="M5" s="216"/>
+      <c r="N5" s="216"/>
+      <c r="O5" s="216"/>
+      <c r="P5" s="216"/>
+      <c r="Q5" s="216"/>
+      <c r="R5" s="216"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -16319,16 +16319,16 @@
       <c r="C7" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="199" t="s">
+      <c r="D7" s="202" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="200"/>
-      <c r="F7" s="200"/>
-      <c r="G7" s="210"/>
-      <c r="H7" s="197">
+      <c r="E7" s="203"/>
+      <c r="F7" s="203"/>
+      <c r="G7" s="217"/>
+      <c r="H7" s="199">
         <v>3</v>
       </c>
-      <c r="I7" s="198"/>
+      <c r="I7" s="201"/>
       <c r="J7" s="7"/>
       <c r="K7" s="3"/>
     </row>
@@ -16351,16 +16351,16 @@
       <c r="C9" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="199" t="s">
+      <c r="D9" s="202" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="200"/>
-      <c r="F9" s="200"/>
-      <c r="G9" s="210"/>
-      <c r="H9" s="197">
+      <c r="E9" s="203"/>
+      <c r="F9" s="203"/>
+      <c r="G9" s="217"/>
+      <c r="H9" s="199">
         <v>4</v>
       </c>
-      <c r="I9" s="198"/>
+      <c r="I9" s="201"/>
       <c r="J9" s="7"/>
       <c r="K9" s="3"/>
     </row>
@@ -16381,16 +16381,16 @@
       <c r="C11" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="199" t="s">
+      <c r="D11" s="202" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="200"/>
-      <c r="F11" s="200"/>
-      <c r="G11" s="201"/>
-      <c r="H11" s="197">
+      <c r="E11" s="203"/>
+      <c r="F11" s="203"/>
+      <c r="G11" s="218"/>
+      <c r="H11" s="199">
         <v>23</v>
       </c>
-      <c r="I11" s="198"/>
+      <c r="I11" s="201"/>
       <c r="J11" s="7"/>
       <c r="K11" s="3"/>
     </row>
@@ -16411,16 +16411,16 @@
       <c r="C13" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="199" t="s">
+      <c r="D13" s="202" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="200"/>
-      <c r="F13" s="200"/>
-      <c r="G13" s="210"/>
-      <c r="H13" s="207">
+      <c r="E13" s="203"/>
+      <c r="F13" s="203"/>
+      <c r="G13" s="217"/>
+      <c r="H13" s="197">
         <v>2</v>
       </c>
-      <c r="I13" s="209"/>
+      <c r="I13" s="198"/>
       <c r="J13" s="7"/>
       <c r="K13" s="3"/>
     </row>
@@ -16428,12 +16428,12 @@
       <c r="A14" s="2"/>
       <c r="B14" s="6"/>
       <c r="C14" s="40"/>
-      <c r="D14" s="199" t="s">
+      <c r="D14" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="200"/>
-      <c r="F14" s="200"/>
-      <c r="G14" s="201"/>
+      <c r="E14" s="203"/>
+      <c r="F14" s="203"/>
+      <c r="G14" s="218"/>
       <c r="J14" s="7"/>
       <c r="K14" s="3"/>
     </row>
@@ -16454,16 +16454,16 @@
       <c r="C16" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="199" t="s">
+      <c r="D16" s="202" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="200"/>
-      <c r="F16" s="200"/>
-      <c r="G16" s="210"/>
-      <c r="H16" s="207">
+      <c r="E16" s="203"/>
+      <c r="F16" s="203"/>
+      <c r="G16" s="217"/>
+      <c r="H16" s="197">
         <v>2</v>
       </c>
-      <c r="I16" s="209"/>
+      <c r="I16" s="198"/>
       <c r="J16" s="7"/>
       <c r="K16" s="3"/>
     </row>
@@ -16471,12 +16471,12 @@
       <c r="A17" s="2"/>
       <c r="B17" s="6"/>
       <c r="C17" s="40"/>
-      <c r="D17" s="199" t="s">
+      <c r="D17" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="200"/>
-      <c r="F17" s="200"/>
-      <c r="G17" s="201"/>
+      <c r="E17" s="203"/>
+      <c r="F17" s="203"/>
+      <c r="G17" s="218"/>
       <c r="J17" s="7"/>
       <c r="K17" s="3"/>
     </row>
@@ -16505,10 +16505,10 @@
       <c r="E19" s="195"/>
       <c r="F19" s="195"/>
       <c r="G19" s="195"/>
-      <c r="H19" s="207">
+      <c r="H19" s="197">
         <v>1</v>
       </c>
-      <c r="I19" s="209"/>
+      <c r="I19" s="198"/>
       <c r="J19" s="93"/>
       <c r="K19" s="3"/>
     </row>
@@ -16516,12 +16516,12 @@
       <c r="A20" s="2"/>
       <c r="B20" s="6"/>
       <c r="C20" s="46"/>
-      <c r="D20" s="199" t="s">
+      <c r="D20" s="202" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="200"/>
-      <c r="F20" s="200"/>
-      <c r="G20" s="201"/>
+      <c r="E20" s="203"/>
+      <c r="F20" s="203"/>
+      <c r="G20" s="218"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="7"/>
@@ -16531,12 +16531,12 @@
       <c r="A21" s="2"/>
       <c r="B21" s="6"/>
       <c r="C21" s="46"/>
-      <c r="D21" s="199" t="s">
+      <c r="D21" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="200"/>
-      <c r="F21" s="200"/>
-      <c r="G21" s="201"/>
+      <c r="E21" s="203"/>
+      <c r="F21" s="203"/>
+      <c r="G21" s="218"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="7"/>
@@ -16557,16 +16557,16 @@
       <c r="C23" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="199" t="s">
+      <c r="D23" s="202" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="200"/>
-      <c r="F23" s="200"/>
-      <c r="G23" s="200"/>
-      <c r="H23" s="207">
+      <c r="E23" s="203"/>
+      <c r="F23" s="203"/>
+      <c r="G23" s="203"/>
+      <c r="H23" s="197">
         <v>1</v>
       </c>
-      <c r="I23" s="209"/>
+      <c r="I23" s="198"/>
       <c r="J23" s="93"/>
       <c r="K23" s="3"/>
     </row>
@@ -16574,12 +16574,12 @@
       <c r="A24" s="2"/>
       <c r="B24" s="6"/>
       <c r="C24" s="40"/>
-      <c r="D24" s="199" t="s">
+      <c r="D24" s="202" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="200"/>
-      <c r="F24" s="200"/>
-      <c r="G24" s="200"/>
+      <c r="E24" s="203"/>
+      <c r="F24" s="203"/>
+      <c r="G24" s="203"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="7"/>
@@ -16604,16 +16604,16 @@
       <c r="C26" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="199" t="s">
+      <c r="D26" s="202" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="200"/>
-      <c r="F26" s="200"/>
-      <c r="G26" s="200"/>
-      <c r="H26" s="197">
+      <c r="E26" s="203"/>
+      <c r="F26" s="203"/>
+      <c r="G26" s="203"/>
+      <c r="H26" s="199">
         <v>2</v>
       </c>
-      <c r="I26" s="198"/>
+      <c r="I26" s="201"/>
       <c r="J26" s="93"/>
       <c r="K26" s="3"/>
     </row>
@@ -16621,12 +16621,12 @@
       <c r="A27" s="2"/>
       <c r="B27" s="6"/>
       <c r="C27" s="35"/>
-      <c r="D27" s="199" t="s">
+      <c r="D27" s="202" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="200"/>
-      <c r="F27" s="200"/>
-      <c r="G27" s="200"/>
+      <c r="E27" s="203"/>
+      <c r="F27" s="203"/>
+      <c r="G27" s="203"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="7"/>
@@ -16650,10 +16650,10 @@
       <c r="E29" s="195"/>
       <c r="F29" s="195"/>
       <c r="G29" s="196"/>
-      <c r="H29" s="197">
+      <c r="H29" s="199">
         <v>1</v>
       </c>
-      <c r="I29" s="198"/>
+      <c r="I29" s="201"/>
       <c r="J29" s="34"/>
       <c r="K29" s="3"/>
     </row>
@@ -16661,12 +16661,12 @@
       <c r="A30" s="2"/>
       <c r="B30" s="33"/>
       <c r="C30" s="103"/>
-      <c r="D30" s="199" t="s">
+      <c r="D30" s="202" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="200"/>
-      <c r="F30" s="200"/>
-      <c r="G30" s="200"/>
+      <c r="E30" s="203"/>
+      <c r="F30" s="203"/>
+      <c r="G30" s="203"/>
       <c r="J30" s="34"/>
       <c r="K30" s="3"/>
     </row>
@@ -16687,14 +16687,14 @@
       <c r="A32" s="2"/>
       <c r="B32" s="5"/>
       <c r="C32" s="37"/>
-      <c r="D32" s="202" t="s">
+      <c r="D32" s="204" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="202"/>
-      <c r="F32" s="202"/>
-      <c r="G32" s="202"/>
-      <c r="H32" s="202"/>
-      <c r="I32" s="202"/>
+      <c r="E32" s="204"/>
+      <c r="F32" s="204"/>
+      <c r="G32" s="204"/>
+      <c r="H32" s="204"/>
+      <c r="I32" s="204"/>
       <c r="J32" s="29"/>
       <c r="K32" s="3"/>
     </row>
@@ -16702,12 +16702,12 @@
       <c r="A33" s="2"/>
       <c r="B33" s="30"/>
       <c r="C33" s="38"/>
-      <c r="D33" s="203"/>
-      <c r="E33" s="203"/>
-      <c r="F33" s="203"/>
-      <c r="G33" s="203"/>
-      <c r="H33" s="203"/>
-      <c r="I33" s="203"/>
+      <c r="D33" s="205"/>
+      <c r="E33" s="205"/>
+      <c r="F33" s="205"/>
+      <c r="G33" s="205"/>
+      <c r="H33" s="205"/>
+      <c r="I33" s="205"/>
       <c r="J33" s="31"/>
       <c r="K33" s="3"/>
     </row>
@@ -16723,13 +16723,13 @@
       <c r="D35" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="218" t="s">
+      <c r="E35" s="212" t="s">
         <v>94</v>
       </c>
-      <c r="F35" s="219"/>
-      <c r="G35" s="219"/>
-      <c r="H35" s="219"/>
-      <c r="I35" s="220"/>
+      <c r="F35" s="213"/>
+      <c r="G35" s="213"/>
+      <c r="H35" s="213"/>
+      <c r="I35" s="214"/>
       <c r="J35" s="7"/>
       <c r="K35" s="3"/>
     </row>
@@ -16737,11 +16737,11 @@
       <c r="A36" s="2"/>
       <c r="B36" s="6"/>
       <c r="D36" s="101"/>
-      <c r="E36" s="207"/>
-      <c r="F36" s="208"/>
-      <c r="G36" s="208"/>
-      <c r="H36" s="208"/>
-      <c r="I36" s="209"/>
+      <c r="E36" s="197"/>
+      <c r="F36" s="215"/>
+      <c r="G36" s="215"/>
+      <c r="H36" s="215"/>
+      <c r="I36" s="198"/>
       <c r="J36" s="93"/>
       <c r="K36" s="3"/>
     </row>
@@ -16763,13 +16763,13 @@
       <c r="D38" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="218" t="s">
+      <c r="E38" s="212" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="219"/>
-      <c r="G38" s="219"/>
-      <c r="H38" s="219"/>
-      <c r="I38" s="220"/>
+      <c r="F38" s="213"/>
+      <c r="G38" s="213"/>
+      <c r="H38" s="213"/>
+      <c r="I38" s="214"/>
       <c r="J38" s="7"/>
       <c r="K38" s="3"/>
     </row>
@@ -17033,13 +17033,13 @@
       <c r="D56" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="E56" s="212" t="s">
+      <c r="E56" s="206" t="s">
         <v>91</v>
       </c>
-      <c r="F56" s="212"/>
-      <c r="G56" s="212"/>
-      <c r="H56" s="212"/>
-      <c r="I56" s="212"/>
+      <c r="F56" s="206"/>
+      <c r="G56" s="206"/>
+      <c r="H56" s="206"/>
+      <c r="I56" s="206"/>
       <c r="K56" s="37"/>
       <c r="L56" s="48"/>
       <c r="M56" s="48"/>
@@ -17058,13 +17058,13 @@
       <c r="B57" s="104"/>
       <c r="C57" s="20"/>
       <c r="D57" s="20"/>
-      <c r="E57" s="213" t="s">
+      <c r="E57" s="207" t="s">
         <v>46</v>
       </c>
-      <c r="F57" s="214"/>
-      <c r="G57" s="214"/>
-      <c r="H57" s="214"/>
-      <c r="I57" s="215"/>
+      <c r="F57" s="208"/>
+      <c r="G57" s="208"/>
+      <c r="H57" s="208"/>
+      <c r="I57" s="209"/>
       <c r="J57" s="20"/>
       <c r="K57" s="3"/>
       <c r="U57" s="7"/>
@@ -17130,7 +17130,7 @@
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="216" t="s">
+      <c r="C59" s="210" t="s">
         <v>50</v>
       </c>
       <c r="D59" s="105">
@@ -17164,7 +17164,7 @@
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="217"/>
+      <c r="C60" s="211"/>
       <c r="D60" s="105">
         <v>2</v>
       </c>
@@ -17596,13 +17596,13 @@
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="6"/>
-      <c r="E77" s="197" t="s">
+      <c r="E77" s="199" t="s">
         <v>95</v>
       </c>
-      <c r="F77" s="221"/>
-      <c r="G77" s="221"/>
-      <c r="H77" s="221"/>
-      <c r="I77" s="198"/>
+      <c r="F77" s="200"/>
+      <c r="G77" s="200"/>
+      <c r="H77" s="200"/>
+      <c r="I77" s="201"/>
       <c r="U77" s="7"/>
       <c r="V77" s="3"/>
     </row>
@@ -17618,27 +17618,27 @@
       <c r="D79" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="E79" s="199" t="s">
+      <c r="E79" s="202" t="s">
         <v>49</v>
       </c>
-      <c r="F79" s="200"/>
-      <c r="G79" s="200"/>
-      <c r="H79" s="200"/>
-      <c r="I79" s="200"/>
-      <c r="J79" s="207">
+      <c r="F79" s="203"/>
+      <c r="G79" s="203"/>
+      <c r="H79" s="203"/>
+      <c r="I79" s="203"/>
+      <c r="J79" s="197">
         <v>8</v>
       </c>
-      <c r="K79" s="209"/>
+      <c r="K79" s="198"/>
       <c r="U79" s="7"/>
       <c r="V79" s="3"/>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="6"/>
-      <c r="E80" s="199"/>
-      <c r="F80" s="200"/>
-      <c r="G80" s="200"/>
-      <c r="H80" s="200"/>
+      <c r="E80" s="202"/>
+      <c r="F80" s="203"/>
+      <c r="G80" s="203"/>
+      <c r="H80" s="203"/>
       <c r="U80" s="7"/>
       <c r="V80" s="3"/>
     </row>
@@ -17655,10 +17655,10 @@
       <c r="G81" s="195"/>
       <c r="H81" s="195"/>
       <c r="I81" s="196"/>
-      <c r="J81" s="207" t="s">
+      <c r="J81" s="197" t="s">
         <v>99</v>
       </c>
-      <c r="K81" s="209"/>
+      <c r="K81" s="198"/>
       <c r="U81" s="7"/>
       <c r="V81" s="3"/>
     </row>
@@ -17723,34 +17723,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E81:I81"/>
-    <mergeCell ref="J81:K81"/>
-    <mergeCell ref="E82:I82"/>
-    <mergeCell ref="E76:I76"/>
-    <mergeCell ref="E77:I77"/>
-    <mergeCell ref="E79:I79"/>
-    <mergeCell ref="J79:K79"/>
-    <mergeCell ref="E80:H80"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="D32:I33"/>
-    <mergeCell ref="E56:I56"/>
-    <mergeCell ref="E57:I57"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="H23:I23"/>
     <mergeCell ref="D29:G29"/>
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="D17:G17"/>
@@ -17767,6 +17739,34 @@
     <mergeCell ref="D26:G26"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="D32:I33"/>
+    <mergeCell ref="E56:I56"/>
+    <mergeCell ref="E57:I57"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E81:I81"/>
+    <mergeCell ref="J81:K81"/>
+    <mergeCell ref="E82:I82"/>
+    <mergeCell ref="E76:I76"/>
+    <mergeCell ref="E77:I77"/>
+    <mergeCell ref="E79:I79"/>
+    <mergeCell ref="J79:K79"/>
+    <mergeCell ref="E80:H80"/>
   </mergeCells>
   <conditionalFormatting sqref="E36:I36 E59:G59 E67:T74 E60:E62 G62:J62 F61:F62 G60:G61 I61:J61 J60 E63:K66 M59:T66">
     <cfRule type="notContainsBlanks" dxfId="8" priority="9">

</xml_diff>